<commit_message>
update formatting, add plotting
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08552296-1E78-AB4C-BF7B-037E4E2E8689}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6053A30C-7DDB-2E4A-8D96-DD925A9972D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="2280" windowWidth="28040" windowHeight="17440" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
-  <si>
-    <t>Class</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Topic</t>
   </si>
@@ -36,16 +33,10 @@
     <t>Do Before Class</t>
   </si>
   <si>
-    <t>Class 1</t>
-  </si>
-  <si>
     <t>Intro</t>
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Class 2</t>
   </si>
   <si>
     <t>Command Line Basics</t>
@@ -67,9 +58,6 @@
 - JVP pp 33-77</t>
   </si>
   <si>
-    <t>Numpy Numeric Data Types</t>
-  </si>
-  <si>
     <t>Pandas: Series &amp; DataFrames</t>
   </si>
   <si>
@@ -109,9 +97,6 @@
     <t>Defensive Programming</t>
   </si>
   <si>
-    <t>https://thepoliticalmethodologist.com/2016/06/06/embrace-your-fallibility-thoughts-on-code-integrity/</t>
-  </si>
-  <si>
     <t>Plotting with plotnine</t>
   </si>
   <si>
@@ -122,11 +107,6 @@
   </si>
   <si>
     <t>Strings</t>
-  </si>
-  <si>
-    <t>- https://docs.python.org/3/tutorial/introduction.html#strings
-- https://realpython.com/python-data-types/#strings
-- Computerphile: https://www.youtube.com/watch?v=MijmeoH9LT4</t>
   </si>
   <si>
     <t>UNSCHEDULED FOR FLEXIBILITY</t>
@@ -204,13 +184,52 @@
   <si>
     <t>- `Setup Python &lt;setup_environment.ipynb&gt;`_
 - `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
+- `Workflow Management &lt;workflow.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Numeric Data Types</t>
+  </si>
+  <si>
+    <t>- `Python Strings &lt;https://docs.python.org/3/tutorial/introduction.html#strings&gt;`_
+- `More Python Strings &lt;https://realpython.com/python-data-types/#strings&gt;`_
+- `Computerphile Unicode &lt;https://www.youtube.com/watch?v=MijmeoH9LT4&gt;`_</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>In-Class Exercise</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_variables_as_pointers.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Plotting in Python &lt;plotting.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -231,14 +250,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -257,23 +268,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,240 +608,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43703</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="71" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="71" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43703</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43710</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43710</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+      <c r="D5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43717</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43717</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43724</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43724</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43731</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43731</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43738</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43738</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43745</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43745</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43752</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>48</v>
+        <v>17</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -827,13 +864,13 @@
         <v>43752</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,39 +878,39 @@
         <v>43759</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43759</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43766</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -881,53 +918,55 @@
         <v>43766</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43773</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43773</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="127" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43780</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -935,96 +974,96 @@
         <v>43724</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43787</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43787</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43794</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43794</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43801</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43801</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43808</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -1032,14 +1071,11 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="D33" s="7"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D20" r:id="rId1" xr:uid="{B03EC4F7-AFC2-314F-BBBC-BCA8B669C90D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add git and github
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B702A37B-7680-4C4E-818A-E35C3D81851E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A7C8F1-BFBB-B547-8A1C-4A8E2F6FB3B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7040" yWindow="3420" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>Topic</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_plotting_part2.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -914,7 +917,9 @@
       <c r="C19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">

</xml_diff>

<commit_message>
fix numpy exercise link
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A69CB20-1FFA-D046-8A56-6321FA5EBE4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F011FE-A713-5448-87C3-6C55B0A296AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="3420" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="3440" yWindow="1820" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
     <t>- `Git and Github &lt;git_and_github.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>-Link &lt;exercises/Exercise_numpy.ipynb&gt;`_</t>
+    <t>`Link &lt;exercises/Exercise_numpy.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -628,7 +628,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
not a mids student added
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F011FE-A713-5448-87C3-6C55B0A296AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA2E5B9-ED4B-BD47-88EE-BAF990A6FBC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="1820" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -628,7 +628,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add pandas views and copies page
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA2E5B9-ED4B-BD47-88EE-BAF990A6FBC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB48D0DE-59EA-6741-8126-25E15BD9B493}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="1820" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="1360" yWindow="460" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
 </t>
   </si>
   <si>
-    <t>- `Python v R: Pointers &lt;python_v_r.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>- WM Chapter 6</t>
   </si>
   <si>
-    <t>- JVP pp 115-139</t>
-  </si>
-  <si>
     <t>- JVP pp 98 - 114</t>
   </si>
   <si>
@@ -239,6 +233,14 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_numpy.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- JVP pp 115-139
+- `Views and Copies in Pandas &lt;views_and_copies_in_pandas.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
+- `Python v R: Pointers &lt;python_v_r.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -628,7 +630,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,7 +646,7 @@
         <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -653,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -661,7 +663,7 @@
         <v>43703</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -675,7 +677,7 @@
         <v>43703</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -684,7 +686,7 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -692,7 +694,7 @@
         <v>43710</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -701,7 +703,7 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -709,33 +711,33 @@
         <v>43710</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43717</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,16 +745,16 @@
         <v>43717</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -760,13 +762,13 @@
         <v>43724</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -774,16 +776,16 @@
         <v>43724</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -791,30 +793,30 @@
         <v>43731</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43731</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -822,13 +824,13 @@
         <v>43738</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -836,13 +838,13 @@
         <v>43738</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -850,7 +852,7 @@
         <v>43745</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -862,13 +864,13 @@
         <v>43745</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -876,13 +878,13 @@
         <v>43752</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -890,13 +892,13 @@
         <v>43752</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -904,13 +906,13 @@
         <v>43759</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -918,13 +920,13 @@
         <v>43759</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -932,13 +934,13 @@
         <v>43766</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -946,13 +948,13 @@
         <v>43766</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -960,13 +962,13 @@
         <v>43773</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -974,13 +976,13 @@
         <v>43773</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -988,13 +990,13 @@
         <v>43780</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="57" x14ac:dyDescent="0.2">
@@ -1002,13 +1004,13 @@
         <v>43724</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1016,7 +1018,7 @@
         <v>43787</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>24</v>
@@ -1028,7 +1030,7 @@
         <v>43787</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>25</v>
@@ -1040,7 +1042,7 @@
         <v>43794</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>26</v>
@@ -1052,7 +1054,7 @@
         <v>43794</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>27</v>
@@ -1064,7 +1066,7 @@
         <v>43801</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>28</v>
@@ -1076,7 +1078,7 @@
         <v>43801</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>29</v>
@@ -1088,7 +1090,7 @@
         <v>43808</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
add first pandas exercise
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB48D0DE-59EA-6741-8126-25E15BD9B493}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52F5CE6-B4DB-804B-BAF3-AEC508E98793}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="460" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>Topic</t>
   </si>
@@ -241,6 +241,9 @@
   <si>
     <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
 - `Python v R: Pointers &lt;python_v_r.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_series_df.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -630,7 +633,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -770,6 +773,9 @@
       <c r="D8" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">

</xml_diff>

<commit_message>
add missing and indices practice
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52F5CE6-B4DB-804B-BAF3-AEC508E98793}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E93816-81E3-4443-AD28-1C0B77096BB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="460" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>Topic</t>
   </si>
@@ -207,10 +207,6 @@
     <t>- `Getting Help &lt;getting_help.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Python Strings &lt;https://docs.python.org/3/tutorial/introduction.html#strings&gt;`_
-- `Computerphile Unicode &lt;https://www.youtube.com/watch?v=MijmeoH9LT4&gt;`_</t>
-  </si>
-  <si>
     <t>Intro to Plotting with PlotNine</t>
   </si>
   <si>
@@ -244,6 +240,13 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_series_df.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Python Strings &lt;https://www.youtube.com/watch?v=pUbfDilfutE&gt;`_
+- `Computerphile Unicode &lt;https://www.youtube.com/watch?v=MijmeoH9LT4&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_indices_missing.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>55</v>
@@ -757,7 +760,7 @@
         <v>56</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -774,7 +777,7 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -785,13 +788,13 @@
         <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>60</v>
-      </c>
       <c r="E9" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -802,13 +805,13 @@
         <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="E10" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="43" x14ac:dyDescent="0.2">
@@ -822,7 +825,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -932,7 +938,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1016,7 +1022,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
split indices and missing, add cleanign exercises.
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E93816-81E3-4443-AD28-1C0B77096BB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0A98F9-14C1-6449-9EF4-51AD50BCD050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="460" windowWidth="31360" windowHeight="16980" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="280" yWindow="1480" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -96,12 +96,6 @@
     <t>Machine Learning with sckikit-learn</t>
   </si>
   <si>
-    <t>Strings</t>
-  </si>
-  <si>
-    <t>UNSCHEDULED FOR FLEXIBILITY</t>
-  </si>
-  <si>
     <t>Data Science: Questions</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>- JVP pp 149 - 157</t>
   </si>
   <si>
-    <t>- WM Chapter 7</t>
-  </si>
-  <si>
     <t>- WM Chapter 6</t>
   </si>
   <si>
@@ -242,11 +233,21 @@
     <t>`Link &lt;exercises/Exercise_series_df.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Python Strings &lt;https://www.youtube.com/watch?v=pUbfDilfutE&gt;`_
-- `Computerphile Unicode &lt;https://www.youtube.com/watch?v=MijmeoH9LT4&gt;`_</t>
-  </si>
-  <si>
-    <t>`Link &lt;exercises/Exercise_indices_missing.ipynb&gt;`_</t>
+    <t>Weighting</t>
+  </si>
+  <si>
+    <t>- WM Chapter 7
+- `Python Strings &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
+  </si>
+  <si>
+    <t>OPEN FOR FLEXIBILITY</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_missing.ipynb&gt;`_
+`Link &lt;exercises/Exercise_indices.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>-`Link &lt;exercises/Exercise_cleaning.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -635,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,14 +646,15 @@
     <col min="2" max="2" width="7.83203125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="50.5" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -661,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -669,7 +671,7 @@
         <v>43703</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -683,16 +685,16 @@
         <v>43703</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -700,16 +702,16 @@
         <v>43710</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -717,16 +719,16 @@
         <v>43710</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
@@ -734,16 +736,16 @@
         <v>43717</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -751,16 +753,16 @@
         <v>43717</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -768,16 +770,16 @@
         <v>43724</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -785,16 +787,16 @@
         <v>43724</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -802,33 +804,33 @@
         <v>43731</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43731</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -836,27 +838,30 @@
         <v>43738</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43738</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>40</v>
+        <v>67</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -864,7 +869,7 @@
         <v>43745</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -876,13 +881,13 @@
         <v>43745</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -890,13 +895,13 @@
         <v>43752</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -904,13 +909,13 @@
         <v>43752</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -918,13 +923,13 @@
         <v>43759</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -932,13 +937,13 @@
         <v>43759</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -946,13 +951,13 @@
         <v>43766</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -960,13 +965,13 @@
         <v>43766</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -974,13 +979,13 @@
         <v>43773</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -988,13 +993,10 @@
         <v>43773</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1002,27 +1004,27 @@
         <v>43780</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43724</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1030,22 +1032,22 @@
         <v>43787</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="7"/>
+        <v>68</v>
+      </c>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43787</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -1054,10 +1056,10 @@
         <v>43794</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D28" s="7"/>
     </row>
@@ -1066,10 +1068,10 @@
         <v>43794</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" s="7"/>
     </row>
@@ -1078,10 +1080,10 @@
         <v>43801</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D30" s="7"/>
     </row>
@@ -1090,10 +1092,10 @@
         <v>43801</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D31" s="7"/>
     </row>
@@ -1102,10 +1104,10 @@
         <v>43808</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="7"/>
     </row>
@@ -1115,7 +1117,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D33" s="7"/>
     </row>

</xml_diff>

<commit_message>
indices and cleaning exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0A98F9-14C1-6449-9EF4-51AD50BCD050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64045F-B623-844F-9CAA-123A99256568}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="1480" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -247,7 +247,7 @@
 `Link &lt;exercises/Exercise_indices.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>-`Link &lt;exercises/Exercise_cleaning.ipynb&gt;`_</t>
+    <t>`Link &lt;exercises/Exercise_cleaning.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -637,7 +637,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
write my own intro to series and dataframes tutorials
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64045F-B623-844F-9CAA-123A99256568}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66E6B64-1CAD-7040-942C-2158E576BA32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="1480" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>Topic</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Numpy Basics</t>
-  </si>
-  <si>
-    <t>Pandas: Series &amp; DataFrames</t>
   </si>
   <si>
     <t>Pandas: Indices &amp; Missing</t>
@@ -148,9 +145,6 @@
     <t>- WM Chapter 6</t>
   </si>
   <si>
-    <t>- JVP pp 98 - 114</t>
-  </si>
-  <si>
     <t>- WM Chapter 13</t>
   </si>
   <si>
@@ -240,14 +234,23 @@
 - `Python Strings &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
   </si>
   <si>
-    <t>OPEN FOR FLEXIBILITY</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_missing.ipynb&gt;`_
 `Link &lt;exercises/Exercise_indices.ipynb&gt;`_</t>
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_cleaning.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Pandas: Series</t>
+  </si>
+  <si>
+    <t>Pandas: DataFrames</t>
+  </si>
+  <si>
+    <t>- `Pandas 1: Series &lt;pandas_series.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Pandas 2: DataFrames &lt;pandas_dataframes.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -636,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,10 +654,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -663,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -671,7 +674,7 @@
         <v>43703</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -685,16 +688,16 @@
         <v>43703</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -702,16 +705,16 @@
         <v>43710</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -719,16 +722,16 @@
         <v>43710</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
@@ -736,16 +739,16 @@
         <v>43717</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -753,16 +756,16 @@
         <v>43717</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -770,33 +773,30 @@
         <v>43724</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43724</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -804,104 +804,107 @@
         <v>43731</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43731</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43738</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="43" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43738</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43745</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43745</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43752</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -909,41 +912,41 @@
         <v>43752</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43759</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43759</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -951,41 +954,41 @@
         <v>43766</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43766</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43773</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>40</v>
+        <v>19</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -993,10 +996,13 @@
         <v>43773</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1004,13 +1010,10 @@
         <v>43780</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1018,13 +1021,13 @@
         <v>43724</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1032,22 +1035,24 @@
         <v>43787</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43787</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -1056,10 +1061,10 @@
         <v>43794</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="7"/>
     </row>
@@ -1068,10 +1073,10 @@
         <v>43794</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="7"/>
     </row>
@@ -1080,10 +1085,10 @@
         <v>43801</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D30" s="7"/>
     </row>
@@ -1092,10 +1097,10 @@
         <v>43801</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" s="7"/>
     </row>
@@ -1104,10 +1109,10 @@
         <v>43808</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="7"/>
     </row>
@@ -1117,7 +1122,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" s="7"/>
     </row>

</xml_diff>

<commit_message>
add real class dates
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3063F491-F538-2347-BD28-396D4D9DFAE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{29F223E7-DB32-354B-BFCB-5F2B36DFF3C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="5660" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="12000" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>FINALS BEGIN DEC 11TH</t>
   </si>
   <si>
-    <t>Week of</t>
-  </si>
-  <si>
     <t xml:space="preserve">- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
 </t>
   </si>
@@ -157,12 +154,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Mon</t>
-  </si>
-  <si>
-    <t>Wed</t>
-  </si>
-  <si>
     <t>In-Class Exercise</t>
   </si>
   <si>
@@ -246,15 +237,24 @@
 - IF did not complete DataCamp: Do Numpy Section</t>
   </si>
   <si>
+    <t>- IPython
+- Python v. R / variables as pointers</t>
+  </si>
+  <si>
+    <t>Tues</t>
+  </si>
+  <si>
+    <t>Thurs</t>
+  </si>
+  <si>
     <t xml:space="preserve">- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
 - Read and sign syllabus
-- Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
+- `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
 - Register for DataCamp
 </t>
   </si>
   <si>
-    <t>- IPython
-- Python v. R / variables as pointers</t>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -644,7 +644,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,10 +658,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -670,15 +670,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>43703</v>
+        <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -689,10 +689,10 @@
     </row>
     <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>43703</v>
+        <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -701,196 +701,196 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>43710</v>
+        <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>43710</v>
+        <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>43717</v>
+        <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>43717</v>
+        <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>43724</v>
+        <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>43724</v>
+        <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>43731</v>
+        <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>43731</v>
+        <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>43738</v>
+        <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>43738</v>
+        <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>43745</v>
+        <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>43745</v>
+        <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
@@ -899,161 +899,161 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>43752</v>
+        <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>43752</v>
+        <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>43759</v>
+        <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>43759</v>
+        <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>43766</v>
+        <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>43766</v>
+        <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>43773</v>
+        <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>43773</v>
+        <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>43724</v>
+        <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>43787</v>
+        <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>43787</v>
+        <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>21</v>
@@ -1062,10 +1062,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>43794</v>
+        <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>22</v>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>43794</v>
+        <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>23</v>
@@ -1086,10 +1086,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>43801</v>
+        <v>43802</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>24</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>43801</v>
+        <v>43804</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>25</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>43808</v>
+        <v>43809</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>26</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>43808</v>
+        <v>43811</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">

</xml_diff>

<commit_message>
update for grad schedule, not undergrad
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{29F223E7-DB32-354B-BFCB-5F2B36DFF3C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFF374E-B683-CC48-9A62-DEE112E088C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2420" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>Topic</t>
   </si>
@@ -54,15 +54,6 @@
     <t>Pandas: Indices &amp; Missing</t>
   </si>
   <si>
-    <t>Pandas: Loading and saving data</t>
-  </si>
-  <si>
-    <t>Pandas: Cleaning</t>
-  </si>
-  <si>
-    <t>Pandas: Merging</t>
-  </si>
-  <si>
     <t>FALL BREAK</t>
   </si>
   <si>
@@ -106,18 +97,12 @@
   </si>
   <si>
     <t>Project Proposal Workshopping</t>
-  </si>
-  <si>
-    <t>FINALS BEGIN DEC 11TH</t>
   </si>
   <si>
     <t xml:space="preserve">- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
 </t>
   </si>
   <si>
-    <t>- `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- WM 12.1
 - JVP pp 208 - 213</t>
   </si>
@@ -131,9 +116,6 @@
     <t>- JVP pp 149 - 157</t>
   </si>
   <si>
-    <t>- WM Chapter 6</t>
-  </si>
-  <si>
     <t>- WM Chapter 13</t>
   </si>
   <si>
@@ -148,9 +130,6 @@
 - `Workflow Management &lt;workflow.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Numeric Data Types</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -201,13 +180,6 @@
 - `Python v R: Pointers &lt;python_v_r.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Weighting</t>
-  </si>
-  <si>
-    <t>- WM Chapter 7
-- `Python Strings &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_missing.ipynb&gt;`_
 `Link &lt;exercises/Exercise_indices.ipynb&gt;`_</t>
   </si>
@@ -233,10 +205,6 @@
     <t>`Link &lt;exercises/Exercise_df.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- JVP pp 33-77
-- IF did not complete DataCamp: Do Numpy Section</t>
-  </si>
-  <si>
     <t>- IPython
 - Python v. R / variables as pointers</t>
   </si>
@@ -247,14 +215,30 @@
     <t>Thurs</t>
   </si>
   <si>
-    <t xml:space="preserve">- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
+    <t>Date</t>
+  </si>
+  <si>
+    <t>- JVP pp 33-77
+- IF did not complete DataCamp: Do Numpy Section
+- `Numbers in Computer &lt;ints_and_floats.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Command Line Basics &lt;command_line_part1.ipynb&gt;`_
 - Read and sign syllabus
 - `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
-- Register for DataCamp
-</t>
-  </si>
-  <si>
-    <t>Date</t>
+- Register for DataCamp</t>
+  </si>
+  <si>
+    <t>- Pandas: Merging</t>
+  </si>
+  <si>
+    <t>- Pandas: Loading and saving data
+- Pandas: Cleaning</t>
+  </si>
+  <si>
+    <t>- WM Chapter 6
+- WM Chapter 7
+- `Python Strings &lt;https://realpython.com/python-data-types/#strings&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -641,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,10 +642,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -670,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -678,7 +662,7 @@
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -687,21 +671,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="71" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -709,16 +693,16 @@
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -726,16 +710,16 @@
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
@@ -743,30 +727,30 @@
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -774,16 +758,16 @@
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -791,16 +775,16 @@
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -808,16 +792,16 @@
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -825,16 +809,16 @@
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="102" x14ac:dyDescent="0.2">
@@ -842,47 +826,47 @@
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>59</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="43" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -890,25 +874,24 @@
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="7"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>11</v>
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -916,13 +899,13 @@
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -930,69 +913,69 @@
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>58</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,13 +983,13 @@
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1014,10 +997,10 @@
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1025,13 +1008,10 @@
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1039,13 +1019,10 @@
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1053,82 +1030,34 @@
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>43802</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>43804</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>43809</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>43811</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="7"/>
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix  dataframe exercise link
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B438AD75-2553-8245-BA74-E7B0F83FD65C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB59CE-594D-6A49-85F5-937D4A178C6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="3660" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2420" yWindow="1500" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -194,9 +194,6 @@
     <t>`Link &lt;exercises/Exercise_series.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>`Link &lt;exercises/Exercise_df.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- IPython
 - Python v. R / variables as pointers</t>
   </si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_variables_v_objects.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_dataframe.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +646,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>33</v>
@@ -666,7 +666,7 @@
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -680,13 +680,13 @@
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>36</v>
@@ -697,7 +697,7 @@
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -714,7 +714,7 @@
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -731,16 +731,16 @@
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" t="s">
         <v>65</v>
-      </c>
-      <c r="E6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43" x14ac:dyDescent="0.2">
@@ -748,13 +748,13 @@
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>46</v>
@@ -765,7 +765,7 @@
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>49</v>
@@ -782,7 +782,7 @@
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>50</v>
@@ -791,7 +791,7 @@
         <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>39</v>
@@ -816,7 +816,7 @@
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>41</v>
@@ -833,13 +833,13 @@
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>47</v>
@@ -850,13 +850,13 @@
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>48</v>
@@ -867,10 +867,10 @@
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>28</v>
@@ -881,7 +881,7 @@
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -892,7 +892,7 @@
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -906,7 +906,7 @@
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
@@ -920,7 +920,7 @@
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
@@ -934,7 +934,7 @@
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>15</v>
@@ -948,7 +948,7 @@
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -962,7 +962,7 @@
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>12</v>
@@ -976,7 +976,7 @@
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>16</v>
@@ -990,7 +990,7 @@
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>17</v>
@@ -1004,7 +1004,7 @@
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>18</v>
@@ -1015,7 +1015,7 @@
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>19</v>
@@ -1026,7 +1026,7 @@
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>21</v>
@@ -1037,7 +1037,7 @@
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>22</v>
@@ -1048,7 +1048,7 @@
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>23</v>
@@ -1060,7 +1060,7 @@
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
add first day materials
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B72106-8FA0-B841-9E49-A9F60F906F6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A58E12-560E-3C49-93E5-9D7AFF69D835}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="1500" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2420" yWindow="1120" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>THANKSGIVING BREAK</t>
   </si>
   <si>
-    <t>Data Science: Backwards Design II</t>
-  </si>
-  <si>
     <t>Data Science: Tool Selection</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
 - Read and sign syllabus
 - `Register with IPUMS &lt;https://uma.pop.umn.edu/usa/user/new&gt;`_
 - `Register for DataCamp &lt;https://www.datacamp.com/home&gt;`_</t>
+  </si>
+  <si>
+    <t>Plaintext Manipulation</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,10 +646,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -666,7 +666,7 @@
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -680,16 +680,16 @@
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -697,16 +697,16 @@
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
@@ -714,16 +714,16 @@
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
@@ -731,16 +731,16 @@
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
         <v>63</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43" x14ac:dyDescent="0.2">
@@ -748,16 +748,16 @@
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -765,16 +765,16 @@
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -782,16 +782,16 @@
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -799,16 +799,16 @@
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="E10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -816,16 +816,16 @@
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -833,16 +833,16 @@
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.2">
@@ -850,16 +850,16 @@
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="E13" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -867,13 +867,13 @@
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -881,7 +881,7 @@
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -892,13 +892,13 @@
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -906,13 +906,13 @@
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -920,13 +920,13 @@
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -934,13 +934,13 @@
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -948,13 +948,13 @@
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.2">
@@ -962,13 +962,13 @@
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -976,13 +976,13 @@
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -990,13 +990,13 @@
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1004,10 +1004,10 @@
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1015,10 +1015,10 @@
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1026,10 +1026,10 @@
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1037,10 +1037,10 @@
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1048,10 +1048,10 @@
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="4"/>
     </row>
@@ -1060,7 +1060,7 @@
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
update class schedule, edit command line 2 exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A58E12-560E-3C49-93E5-9D7AFF69D835}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44A5BF8E-122D-9744-805E-A42FC5BA1425}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="1120" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="4900" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Topic</t>
   </si>
@@ -42,12 +42,6 @@
     <t>Command Line Basics</t>
   </si>
   <si>
-    <t>Advanced Command Line</t>
-  </si>
-  <si>
-    <t>Jupyter Lab / Notebooks</t>
-  </si>
-  <si>
     <t>Numpy Basics</t>
   </si>
   <si>
@@ -94,10 +88,6 @@
   </si>
   <si>
     <t>Project Proposal Workshopping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
-</t>
   </si>
   <si>
     <t>- WM 12.1
@@ -119,10 +109,6 @@
     <t>- JVP pp 331 - 359</t>
   </si>
   <si>
-    <t>- `Setup Python &lt;setup_environment.ipynb&gt;`_
-- `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
 - `Workflow Management &lt;workflow.ipynb&gt;`_</t>
   </si>
@@ -133,13 +119,7 @@
     <t>In-Class Exercise</t>
   </si>
   <si>
-    <t>`Link &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>`Link &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_</t>
   </si>
   <si>
     <t>- `Getting Help &lt;getting_help.ipynb&gt;`_</t>
@@ -243,6 +223,26 @@
   </si>
   <si>
     <t>Plaintext Manipulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- `Advanced Command Line &lt;command_line_part2.ipynb&gt;`_
+- `Setup Python &lt;setup_environment.ipynb&gt;`_
+- `Jupyter Tutorial &lt;jupyter.ipynb&gt;`_
+</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_CommandLine_2_Advanced.ipynb&gt;`_
+`Link 2 &lt;exercises/Exercise_jupyterlab.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Rm</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>- Advanced Command Line
+- Jupyter Lab / Notebooks</t>
   </si>
 </sst>
 </file>
@@ -629,441 +629,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="8" customWidth="1"/>
-    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="2" max="3" width="7.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="50.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3">
+        <v>270</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+      <c r="E3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="C4" s="3">
+        <v>270</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="71" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="71" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3">
+        <v>330</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3">
+        <v>330</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3">
+        <v>330</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3">
+        <v>330</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="F11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3">
+        <v>270</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="F12" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="C13" s="3">
+        <v>330</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C14" s="3">
+        <v>270</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3">
+        <v>330</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C16" s="3">
+        <v>270</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="3">
+        <v>330</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3">
+        <v>330</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="E18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3">
+        <v>330</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C20" s="3">
+        <v>270</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C21" s="3">
+        <v>330</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C22" s="3">
+        <v>270</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C23" s="3">
+        <v>330</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C24" s="3">
+        <v>330</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3">
+        <v>330</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3">
+        <v>270</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="C27" s="3">
+        <v>330</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="C28" s="3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>20</v>
+        <v>49</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update series exercises and jupyter lab data
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44A5BF8E-122D-9744-805E-A42FC5BA1425}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74326E3-1C29-1649-AE9D-2F100AA67BAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4900" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="2420" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
   <si>
     <t>Topic</t>
   </si>
@@ -243,6 +243,9 @@
   <si>
     <t>- Advanced Command Line
 - Jupyter Lab / Notebooks</t>
+  </si>
+  <si>
+    <t>Big Data: What is it, how do I work with it?</t>
   </si>
 </sst>
 </file>
@@ -631,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,7 +1062,7 @@
         <v>330</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1073,7 +1076,7 @@
         <v>330</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1087,7 +1090,7 @@
         <v>330</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1101,7 +1104,7 @@
         <v>270</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1115,7 +1118,7 @@
         <v>330</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27" s="4"/>
     </row>
@@ -1128,6 +1131,9 @@
       </c>
       <c r="C28" s="3">
         <v>270</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update bash on windows and other install directions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74326E3-1C29-1649-AE9D-2F100AA67BAB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7363747-22F0-6F46-9AAC-7357B820F965}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -171,10 +171,6 @@
     <t>`Link &lt;exercises/Exercise_series.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- IPython
-- Python v. R / variables as pointers</t>
-  </si>
-  <si>
     <t>Tues</t>
   </si>
   <si>
@@ -204,10 +200,6 @@
     <t>- WM pp 136-142
 - JVP pp 115-139
 - `Views and Copies in Pandas &lt;views_and_copies_in_pandas.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
-- `variables v objects &lt;python_v_r.ipynb&gt;`_</t>
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_variables_v_objects.ipynb&gt;`_</t>
@@ -246,6 +238,16 @@
   </si>
   <si>
     <t>Big Data: What is it, how do I work with it?</t>
+  </si>
+  <si>
+    <t>- Ipython
+- Packages
+- Python v. R / variables as pointers</t>
+  </si>
+  <si>
+    <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
+- `Python packages &lt;managing_python_packages.ipynb&gt;`_
+- `variables v objects &lt;python_v_r.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -634,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,13 +651,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -672,7 +674,7 @@
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3">
         <v>270</v>
@@ -689,16 +691,16 @@
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
@@ -709,39 +711,39 @@
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3">
         <v>270</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="71" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43" x14ac:dyDescent="0.2">
@@ -749,7 +751,7 @@
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3">
         <v>330</v>
@@ -758,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>39</v>
@@ -769,7 +771,7 @@
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3">
         <v>330</v>
@@ -789,10 +791,10 @@
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>43</v>
@@ -801,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -809,10 +811,10 @@
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>32</v>
@@ -829,7 +831,7 @@
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3">
         <v>330</v>
@@ -849,7 +851,7 @@
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3">
         <v>330</v>
@@ -858,7 +860,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>40</v>
@@ -869,16 +871,16 @@
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3">
         <v>270</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>41</v>
@@ -889,13 +891,13 @@
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3">
         <v>330</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>24</v>
@@ -906,7 +908,7 @@
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3">
         <v>270</v>
@@ -923,7 +925,7 @@
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3">
         <v>330</v>
@@ -937,7 +939,7 @@
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3">
         <v>270</v>
@@ -954,7 +956,7 @@
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="3">
         <v>330</v>
@@ -971,7 +973,7 @@
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3">
         <v>330</v>
@@ -988,7 +990,7 @@
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3">
         <v>330</v>
@@ -1005,7 +1007,7 @@
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="3">
         <v>270</v>
@@ -1022,7 +1024,7 @@
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="3">
         <v>330</v>
@@ -1039,7 +1041,7 @@
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3">
         <v>270</v>
@@ -1056,13 +1058,13 @@
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3">
         <v>330</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1070,13 +1072,13 @@
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3">
         <v>330</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1084,7 +1086,7 @@
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3">
         <v>330</v>
@@ -1098,7 +1100,7 @@
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="3">
         <v>270</v>
@@ -1112,7 +1114,7 @@
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="3">
         <v>330</v>
@@ -1127,7 +1129,7 @@
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="3">
         <v>270</v>
@@ -1141,7 +1143,7 @@
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">

</xml_diff>

<commit_message>
add build with merging exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30B6B468-E704-E942-846F-35C9D22ED087}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2B7FDC-C2A3-3C47-B5C5-558883B92D1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2420" yWindow="460" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>Topic</t>
   </si>
@@ -248,6 +248,9 @@
     <t>- `Follow this link &lt;https://gke.mybinder.org/v2/gh/ipython/ipython-in-depth/master?filepath=binder/Index.ipynb&gt;`_ , then click "Ipython - Beyond plain python" and read that notebook. 
 - `Python packages &lt;managing_python_packages.ipynb&gt;`_
 - `variables v objects &lt;vars_v_objects.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_merging.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,6 +905,9 @@
       <c r="E13" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="F13" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">

</xml_diff>

<commit_message>
fix up dataframe exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A1DBBF-5C23-434F-BFD3-215C0BDE5D9F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF3BBCA-037E-9748-BF3D-51A3020F0E91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17000" yWindow="5140" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="1920" yWindow="2900" windowWidth="35980" windowHeight="18880" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>Topic</t>
   </si>
@@ -262,6 +262,9 @@
   </si>
   <si>
     <t>- JVP pp 212-228</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_groupby.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -650,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,6 +973,9 @@
       <c r="E16" s="10" t="s">
         <v>68</v>
       </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">

</xml_diff>

<commit_message>
update course schedule for parallelism and big data
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BB4967-A15D-7A41-8C16-5677106165A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD2425-0623-BE46-A2D6-77DDD2959238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="460" windowWidth="25600" windowHeight="14560" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="10960" yWindow="460" windowWidth="25780" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>Topic</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>Collaborating using Github</t>
-  </si>
-  <si>
-    <t>Getting Help Online</t>
-  </si>
-  <si>
-    <t>Defensive Programming</t>
   </si>
   <si>
     <t>Statistics with statsmodels</t>
@@ -106,10 +100,6 @@
     <t>- JVP pp 331 - 359</t>
   </si>
   <si>
-    <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
-- `Workflow Management &lt;workflow.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -117,9 +107,6 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_CommandLine_1_Basics.ipynb&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Getting Help &lt;getting_help.ipynb&gt;`_</t>
   </si>
   <si>
     <t>Intro to Plotting with PlotNine</t>
@@ -268,6 +255,25 @@
   <si>
     <t>`Link 1&lt;exercises/Exercise_indices.ipynb&gt;`_
 `Link 2&lt;exercises/Exercise_missing.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
+- `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- Defensive Programming
+- Getting Help Online</t>
+  </si>
+  <si>
+    <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
+- `Workflow Management &lt;workflow.ipynb&gt;`_
+- `Getting Help &lt;getting_help.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Parallel Computing</t>
+  </si>
+  <si>
+    <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -656,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,13 +677,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -686,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -694,7 +700,7 @@
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C2" s="3">
         <v>270</v>
@@ -711,19 +717,19 @@
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -731,19 +737,19 @@
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3">
         <v>270</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -751,19 +757,19 @@
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3">
         <v>270</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43" x14ac:dyDescent="0.2">
@@ -771,7 +777,7 @@
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3">
         <v>330</v>
@@ -780,10 +786,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -791,19 +797,19 @@
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3">
         <v>270</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
         <v>38</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -811,19 +817,19 @@
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -831,19 +837,19 @@
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -851,19 +857,19 @@
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3">
         <v>330</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -871,7 +877,7 @@
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" s="3">
         <v>270</v>
@@ -880,10 +886,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -891,19 +897,19 @@
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3">
         <v>270</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -911,19 +917,19 @@
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3">
         <v>330</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="99" x14ac:dyDescent="0.2">
@@ -931,7 +937,7 @@
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3">
         <v>270</v>
@@ -940,10 +946,10 @@
         <v>8</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -951,7 +957,7 @@
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3">
         <v>330</v>
@@ -965,19 +971,19 @@
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3">
         <v>270</v>
       </c>
       <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -985,7 +991,7 @@
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17" s="3">
         <v>330</v>
@@ -994,58 +1000,58 @@
         <v>10</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="3">
         <v>330</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>12</v>
+      <c r="D18" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3">
         <v>330</v>
       </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+      <c r="D19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3">
         <v>270</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>20</v>
@@ -1056,33 +1062,33 @@
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3">
         <v>330</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3">
         <v>270</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>23</v>
+        <v>55</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1090,27 +1096,30 @@
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3">
         <v>330</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3">
         <v>330</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1118,13 +1127,13 @@
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3">
         <v>330</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1132,13 +1141,13 @@
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" s="3">
         <v>270</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1146,13 +1155,13 @@
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C27" s="3">
         <v>330</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E27" s="4"/>
     </row>
@@ -1161,13 +1170,13 @@
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3">
         <v>270</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1175,11 +1184,11 @@
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix schedule format issue
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CD2425-0623-BE46-A2D6-77DDD2959238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECB07ED-22C8-5940-AAA6-7BDE3949C823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10960" yWindow="460" windowWidth="25780" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -253,10 +253,6 @@
     <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>`Link 1&lt;exercises/Exercise_indices.ipynb&gt;`_
-`Link 2&lt;exercises/Exercise_missing.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
 - `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_</t>
   </si>
@@ -274,6 +270,10 @@
   </si>
   <si>
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
+- `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,7 +889,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -1017,10 +1017,10 @@
         <v>330</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.2">
@@ -1088,7 +1088,7 @@
         <v>55</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1116,10 +1116,10 @@
         <v>330</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add big data, fix indices exercise typos
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECB07ED-22C8-5940-AAA6-7BDE3949C823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D680C703-EB05-604A-9414-3038DB87A4A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10960" yWindow="460" windowWidth="25780" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
-    <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
+    <sheet name="class_schedule_xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>Topic</t>
   </si>
@@ -241,9 +241,6 @@
 - `What is goal of reshaping? &lt;https://www.jstatsoft.org/index.php/jss/article/view/v059i10/v59i10.pdf&gt;`_</t>
   </si>
   <si>
-    <t>Speed and Performance in Python</t>
-  </si>
-  <si>
     <t>- JVP pp 212-228</t>
   </si>
   <si>
@@ -266,14 +263,15 @@
 - `Getting Help &lt;getting_help.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Parallel Computing</t>
-  </si>
-  <si>
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
-- `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
+    <t>`Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
+`Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- Speed and Performance in Python
+- Parallelism</t>
   </si>
 </sst>
 </file>
@@ -662,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,7 +887,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -980,10 +978,10 @@
         <v>59</v>
       </c>
       <c r="E16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
         <v>63</v>
-      </c>
-      <c r="F16" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1003,10 +1001,10 @@
         <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
@@ -1016,11 +1014,11 @@
       <c r="C18" s="3">
         <v>330</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>68</v>
+      <c r="D18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.2">
@@ -1033,14 +1031,14 @@
       <c r="C19" s="3">
         <v>330</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43767</v>
       </c>
@@ -1050,14 +1048,14 @@
       <c r="C20" s="3">
         <v>270</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43769</v>
       </c>
@@ -1068,13 +1066,13 @@
         <v>330</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43774</v>
       </c>
@@ -1085,10 +1083,10 @@
         <v>270</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>66</v>
+        <v>11</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1102,10 +1100,13 @@
         <v>330</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43781</v>
       </c>
@@ -1115,12 +1116,7 @@
       <c r="C24" s="3">
         <v>330</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">

</xml_diff>

<commit_message>
update performance to be two pages
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A9C4AC7-45A7-004A-902A-20A447245AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{93008678-4F3F-0E4B-A9AA-E4D443484223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="460" windowWidth="25780" windowHeight="19620" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="10960" yWindow="460" windowWidth="25780" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -276,7 +276,8 @@
     <t>Parallelism</t>
   </si>
   <si>
-    <t xml:space="preserve"> - `Performance &lt;performance.ipynb&gt;`_</t>
+    <t xml:space="preserve"> - `Understanding Performance &lt;performance_understanding.ipynb&gt;`_
+ - `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1027,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43762</v>
       </c>

</xml_diff>

<commit_message>
fix class schedule, update performance
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8F38069A-B397-2E45-9308-56293DA41248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCA5D1B-FAC5-F243-89CF-E9CF00FB77B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10960" yWindow="460" windowWidth="25780" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="12160" yWindow="2080" windowWidth="25780" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -276,8 +276,8 @@
     <t>Parallelism</t>
   </si>
   <si>
-    <t xml:space="preserve"> - `Understanding Performance &lt;performance_understanding.ipynb&gt;`_
- - `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
+    <t>- `Understanding Performance &lt;performance_understanding.ipynb&gt;`_
+- `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,27 +936,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="3">
-        <v>270</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43748</v>
       </c>
@@ -966,8 +958,14 @@
       <c r="C15" s="3">
         <v>330</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
+      <c r="D15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update big data exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCA5D1B-FAC5-F243-89CF-E9CF00FB77B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3AA6302-3CFF-8749-B430-B418E663F051}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12160" yWindow="2080" windowWidth="25780" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>Topic</t>
   </si>
@@ -250,10 +250,6 @@
     <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
-- `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- Defensive Programming
 - Getting Help Online</t>
   </si>
@@ -278,6 +274,14 @@
   <si>
     <t>- `Understanding Performance &lt;performance_understanding.ipynb&gt;`_
 - `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
+- `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_
+- Download the dataset linked at the top of the linked exercise.</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -666,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,7 +897,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -1008,7 +1012,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
@@ -1022,7 +1026,10 @@
         <v>55</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>65</v>
+        <v>72</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -1036,10 +1043,10 @@
         <v>330</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1053,10 +1060,10 @@
         <v>270</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -1070,10 +1077,10 @@
         <v>330</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update project summary with final product details
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{34183BEB-03F0-4D44-868B-C7CC38B3CC39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03D1C85-6739-D044-AF78-2695CF2FC3E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12160" yWindow="2080" windowWidth="25780" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -671,7 +671,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,7 +952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43748</v>
       </c>
@@ -962,17 +962,17 @@
       <c r="C15" s="3">
         <v>330</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>8</v>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43753</v>
       </c>
@@ -982,17 +982,17 @@
       <c r="C16" s="3">
         <v>270</v>
       </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43755</v>
       </c>
@@ -1002,17 +1002,17 @@
       <c r="C17" s="3">
         <v>330</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
+      <c r="D17" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="F17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
@@ -1022,14 +1022,14 @@
       <c r="C18" s="3">
         <v>330</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>73</v>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="68" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update schedule and project summary
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647385CD-14A1-3D4D-A325-90B2CE2DB091}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6AAF65-9AF8-2644-95FA-54362741D602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="26380" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t>Topic</t>
   </si>
@@ -250,10 +250,6 @@
     <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- Defensive Programming
-- Getting Help Online</t>
-  </si>
-  <si>
     <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
 - `Workflow Management &lt;workflow.ipynb&gt;`_
 - `Getting Help &lt;getting_help.ipynb&gt;`_</t>
@@ -276,12 +272,20 @@
 - `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
   </si>
   <si>
+    <t>`Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>[Discuss mid-semester project in class]</t>
+  </si>
+  <si>
+    <t>- Defensive Programming
+- Workflow
+- Getting Help Online</t>
+  </si>
+  <si>
     <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
 - `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_
-- Download the dataset linked at the top of the linked exercise.</t>
-  </si>
-  <si>
-    <t>`Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
+- Download the dataset linked at the top of the linked exercise before class.</t>
   </si>
 </sst>
 </file>
@@ -671,7 +675,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,7 +901,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -986,13 +990,13 @@
         <v>55</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43755</v>
       </c>
@@ -1002,17 +1006,17 @@
       <c r="C17" s="3">
         <v>330</v>
       </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>62</v>
+      <c r="D17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
@@ -1022,11 +1026,14 @@
       <c r="C18" s="3">
         <v>330</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>66</v>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="99" x14ac:dyDescent="0.2">
@@ -1060,10 +1067,10 @@
         <v>270</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1077,10 +1084,10 @@
         <v>330</v>
       </c>
       <c r="D21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
completely rework github exercise
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6AAF65-9AF8-2644-95FA-54362741D602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FF526D2-AE0A-8A4A-A092-1ECBDED2C0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6400" yWindow="460" windowWidth="26380" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>THANKSGIVING BREAK</t>
   </si>
   <si>
-    <t>Data Science: Tool Selection</t>
-  </si>
-  <si>
     <t>Project Proposal Workshopping</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>`Link &lt;exercises/Exercise_groupby.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>- `Defensive Programming &lt;defensive_programming.ipynb&gt;`_
 - `Workflow Management &lt;workflow.ipynb&gt;`_
 - `Getting Help &lt;getting_help.ipynb&gt;`_</t>
@@ -286,6 +280,13 @@
     <t>- `What is Big Data? &lt;what_is_big_data.ipynb&gt;`_
 - `Strategies for Big Data &lt;big_data_strategies.ipynb&gt;`_
 - Download the dataset linked at the top of the linked exercise before class.</t>
+  </si>
+  <si>
+    <t>Git and Github 2</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_git.ipynb&gt;`_
+`Link &lt;exercises/Exercise_git_2.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -675,7 +676,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,13 +690,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -704,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -712,7 +713,7 @@
         <v>43704</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3">
         <v>270</v>
@@ -729,19 +730,19 @@
         <v>43706</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -749,19 +750,19 @@
         <v>43711</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3">
         <v>270</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -769,19 +770,19 @@
         <v>43713</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3">
         <v>270</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43" x14ac:dyDescent="0.2">
@@ -789,7 +790,7 @@
         <v>43718</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3">
         <v>330</v>
@@ -798,10 +799,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -809,19 +810,19 @@
         <v>43720</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3">
         <v>270</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -829,19 +830,19 @@
         <v>43725</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -849,19 +850,19 @@
         <v>43727</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>26</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -869,19 +870,19 @@
         <v>43732</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3">
         <v>330</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="F10" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -889,7 +890,7 @@
         <v>43734</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3">
         <v>270</v>
@@ -898,10 +899,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.2">
@@ -909,19 +910,19 @@
         <v>43739</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3">
         <v>270</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -929,19 +930,19 @@
         <v>43741</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3">
         <v>330</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -949,19 +950,19 @@
         <v>43746</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43748</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3">
         <v>330</v>
@@ -970,30 +971,24 @@
         <v>10</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43753</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3">
         <v>270</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>71</v>
+      <c r="D16" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -1001,127 +996,130 @@
         <v>43755</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3">
         <v>330</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="D17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43760</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3">
         <v>330</v>
       </c>
-      <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>62</v>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43762</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3">
         <v>330</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43767</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="3">
         <v>270</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43769</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3">
         <v>330</v>
       </c>
-      <c r="D21" t="s">
-        <v>69</v>
+      <c r="D21" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43774</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3">
         <v>270</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43776</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="3">
         <v>330</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1129,16 +1127,16 @@
         <v>43781</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="3">
         <v>330</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1146,13 +1144,16 @@
         <v>43783</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="3">
         <v>330</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1160,13 +1161,13 @@
         <v>43788</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3">
         <v>270</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1174,28 +1175,27 @@
         <v>43790</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3">
         <v>330</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43795</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3">
         <v>270</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1203,7 +1203,7 @@
         <v>43797</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">

</xml_diff>

<commit_message>
finish big data exercises and solutions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FF526D2-AE0A-8A4A-A092-1ECBDED2C0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2889860F-C446-C947-8DDD-6BC12CCE83A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6400" yWindow="460" windowWidth="26380" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -676,7 +676,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
lots of progress on parallelism, update course schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A9AD0522-C351-4C4F-9063-E7B2EDC995D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F82523B-22E1-AB4F-BAB9-4EC75709A1D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="460" windowWidth="30140" windowHeight="19640" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="12040" yWindow="460" windowWidth="30140" windowHeight="19620" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Topic</t>
   </si>
@@ -57,12 +57,6 @@
     <t>FALL BREAK</t>
   </si>
   <si>
-    <t>Pandas: Reshaping</t>
-  </si>
-  <si>
-    <t>Pandas: Categorical Data; Eval and Query</t>
-  </si>
-  <si>
     <t>Collaborating using Github</t>
   </si>
   <si>
@@ -82,10 +76,6 @@
   </si>
   <si>
     <t>Project Proposal Workshopping</t>
-  </si>
-  <si>
-    <t>- WM 12.1
-- JVP pp 208 - 213</t>
   </si>
   <si>
     <t>- JVP pp 149 - 157</t>
@@ -215,11 +205,6 @@
     <t>`Link &lt;exercises/Exercise_reshaping.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- WM 8.3
-- `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_
-- `What is goal of reshaping? &lt;https://www.jstatsoft.org/index.php/jss/article/view/v059i10/v59i10.pdf&gt;`_</t>
-  </si>
-  <si>
     <t>- JVP pp 212-228</t>
   </si>
   <si>
@@ -238,14 +223,7 @@
 `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Speed and Performance in Python</t>
-  </si>
-  <si>
     <t>Parallelism</t>
-  </si>
-  <si>
-    <t>- `Understanding Performance &lt;performance_understanding.ipynb&gt;`_
-- `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
@@ -274,88 +252,108 @@
     <t>Date, Rm</t>
   </si>
   <si>
-    <t>Thurs, Aug 29, rm CC</t>
-  </si>
-  <si>
-    <t>Tues, Sep 03, rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 05, rm 270</t>
-  </si>
-  <si>
-    <t>Tues, Sep 10, rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 12, rm 270</t>
-  </si>
-  <si>
-    <t>Tues, Sep 17, rm CC</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 19, rm CC</t>
-  </si>
-  <si>
-    <t>Tues, Sep 24, rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Sep 26, rm 270</t>
-  </si>
-  <si>
-    <t>Tues, Oct 01, rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 03, rm 330</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tues, Oct 08, rm </t>
-  </si>
-  <si>
-    <t>Thurs, Oct 10, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Oct 15, rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 17, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Oct 22, rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 24, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Oct 29, rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Oct 31, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Nov 05, rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 07, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Nov 12, rm 330</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 14, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Nov 19, rm 270</t>
-  </si>
-  <si>
-    <t>Thurs, Nov 21, rm 330</t>
-  </si>
-  <si>
-    <t>Tues, Nov 26, rm 270</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thurs, Nov 28, rm </t>
-  </si>
-  <si>
-    <t>Tues, Aug 27, rm 270</t>
+    <t>Tues, Aug 27, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Aug 29, Rm CC</t>
+  </si>
+  <si>
+    <t>Tues, Sep 03, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 05, Rm 270</t>
+  </si>
+  <si>
+    <t>Tues, Sep 10, Rm 330</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 12, Rm 270</t>
+  </si>
+  <si>
+    <t>Tues, Sep 17, Rm CC</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 19, Rm CC</t>
+  </si>
+  <si>
+    <t>Tues, Sep 24, Rm 330</t>
+  </si>
+  <si>
+    <t>Thurs, Sep 26, Rm 270</t>
+  </si>
+  <si>
+    <t>Tues, Oct 01, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 03, Rm 330</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tues, Oct 08, Rm </t>
+  </si>
+  <si>
+    <t>Thurs, Oct 10, Rm 330</t>
+  </si>
+  <si>
+    <t>Tues, Oct 15, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 17, Rm 330</t>
+  </si>
+  <si>
+    <t>Tues, Oct 22, Rm 330</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 24, Rm 330</t>
+  </si>
+  <si>
+    <t>Tues, Oct 29, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Oct 31, Rm 330</t>
+  </si>
+  <si>
+    <t>Speed and PerfoRmance in Python</t>
+  </si>
+  <si>
+    <t>- `Understanding PerfoRmance &lt;perfoRmance_understanding.ipynb&gt;`_
+- `Improving PerfoRmance &lt;perfoRmance_solutions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>Tues, Nov 05, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 07, Rm 330</t>
+  </si>
+  <si>
+    <t>Tues, Nov 12, Rm 330</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 14, Rm 330</t>
+  </si>
+  <si>
+    <t>Tues, Nov 19, Rm 270</t>
+  </si>
+  <si>
+    <t>Thurs, Nov 21, Rm 330</t>
+  </si>
+  <si>
+    <t>Tues, Nov 26, Rm 270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thurs, Nov 28, Rm </t>
+  </si>
+  <si>
+    <t>- Pandas: Reshaping
+- Pandas: Categoricals</t>
+  </si>
+  <si>
+    <t>- WM 8.3
+- `Pandas reshaping (with pics!) &lt;https://pandas.pydata.org/pandas-docs/stable/user_guide/reshaping.html&gt;`_
+- `What is goal of reshaping? &lt;https://www.jstatsoft.org/index.php/jss/article/view/v059i10/v59i10.pdf&gt;`_
+- Categoricals: WM 12.1</t>
+  </si>
+  <si>
+    <t>Data Science: Tool Selection</t>
   </si>
 </sst>
 </file>
@@ -744,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,7 +756,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -767,12 +765,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -783,161 +781,161 @@
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -945,167 +943,164 @@
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="99" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>8</v>
+        <v>82</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update reading assignment for thursday
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B778EBF6-0649-C04C-AEB5-EF7F29F7249A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6094B298-6B8B-824B-8076-E6A83EB59926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="460" windowWidth="30140" windowHeight="19620" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="10420" yWindow="460" windowWidth="30140" windowHeight="19620" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>`Link &lt;exercises/Exercise_reshaping.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- JVP pp 212-228</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_groupby.ipynb&gt;`_</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   <si>
     <t>- `Understanding Performance &lt;performance_understanding.ipynb&gt;`_
 - `Improving Performance &lt;performance_solutions.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- WM pp Chpt 10, 10.1, 10.2, 10.3</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,7 +756,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>44</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>46</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>29</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>30</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>20</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
@@ -902,12 +902,12 @@
         <v>38</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>36</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -952,68 +952,68 @@
         <v>26</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
         <v>51</v>
-      </c>
-      <c r="D19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
@@ -1021,29 +1021,29 @@
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>9</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>11</v>
@@ -1073,15 +1073,15 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>14</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
fix schedule with new exercise links
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70A7320-C6E1-1E4B-B0A2-75561FFCC4B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53E41A-0ECF-A046-8659-865C4A88C008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3620" yWindow="460" windowWidth="30140" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Topic</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>[finish groupby and reshaping exercises]</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_scikit_learn.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -752,7 +755,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,6 +1069,9 @@
       <c r="C23" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">

</xml_diff>

<commit_message>
add code your own linear regression
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53E41A-0ECF-A046-8659-865C4A88C008}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3610738-F5F9-0A4D-936E-CE3AEABFC344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3620" yWindow="460" windowWidth="30140" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>Topic</t>
   </si>
@@ -210,9 +210,6 @@
 - `Getting Help &lt;getting_help.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_</t>
-  </si>
-  <si>
     <t>`Link 1 &lt;exercises/Exercise_indices.ipynb&gt;`_
 `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
   </si>
@@ -366,6 +363,14 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_scikit_learn.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_codeyourownlinearregression.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
+- Review Linear Regression Matrix Algebra
+- Review Defining Classes</t>
   </si>
 </sst>
 </file>
@@ -755,7 +760,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,7 +773,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -782,7 +787,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -793,7 +798,7 @@
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -807,7 +812,7 @@
     </row>
     <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>43</v>
@@ -821,7 +826,7 @@
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>45</v>
@@ -835,7 +840,7 @@
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
@@ -849,7 +854,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>28</v>
@@ -863,7 +868,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>29</v>
@@ -877,7 +882,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
@@ -891,7 +896,7 @@
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
@@ -905,7 +910,7 @@
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
@@ -914,12 +919,12 @@
         <v>37</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>35</v>
@@ -933,7 +938,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>34</v>
@@ -947,7 +952,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -955,7 +960,7 @@
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -964,54 +969,54 @@
         <v>25</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
         <v>50</v>
@@ -1019,13 +1024,13 @@
     </row>
     <row r="20" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="D20" t="s">
         <v>49</v>
@@ -1033,35 +1038,35 @@
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>94</v>
-      </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
         <v>96</v>
-      </c>
-      <c r="D22" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
@@ -1070,23 +1075,26 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>11</v>
@@ -1094,15 +1102,15 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>12</v>
@@ -1110,7 +1118,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>14</v>
@@ -1118,7 +1126,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add dask intro, update schedule
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D45DE7-0308-AC4D-9CEB-63C9F5518F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6C9CFF-3A28-A348-9F31-AC288E50DF9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="460" windowWidth="30140" windowHeight="19580" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Topic</t>
   </si>
@@ -66,16 +66,7 @@
     <t>Machine Learning with sckikit-learn</t>
   </si>
   <si>
-    <t>Data Science: Questions</t>
-  </si>
-  <si>
-    <t>Data Science: Backwards Design</t>
-  </si>
-  <si>
     <t>THANKSGIVING BREAK</t>
-  </si>
-  <si>
-    <t>Project Proposal Workshopping</t>
   </si>
   <si>
     <t>- JVP pp 149 - 157</t>
@@ -214,9 +205,6 @@
 `Link 2 &lt;exercises/Exercise_missing.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>Parallelism</t>
-  </si>
-  <si>
     <t>`Link &lt;exercises/Exercise_bigdata.ipynb&gt;`_</t>
   </si>
   <si>
@@ -365,12 +353,37 @@
     <t>`Link &lt;exercises/Exercise_codeyourownlinearregression.ipynb&gt;`_</t>
   </si>
   <si>
+    <t>Statsmodels Day 2</t>
+  </si>
+  <si>
+    <t>Regular Expressions</t>
+  </si>
+  <si>
+    <t>- `Regular Expressions Tutorial &lt;https://scotch.io/tutorials/an-introduction-to-regex-in-python&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Parallel ML with Dask &lt;https://www.youtube.com/watch?v=tQBovBvSDvA&amp;list=PLsT4-aZA6_bgaRhsc0JaZXSi5kt-RIJgQ&gt;`_
+- `What is Dask? &lt;scaling_parallelism_and_distributedcomputing.ipynb&gt;`_
+- `OPTIONAL: Full Dask Tutorial (3+ Hours) &lt;https://www.youtube.com/watch?v=mqdglv9GnM8&amp;list=PLsT4-aZA6_bgaRhsc0JaZXSi5kt-RIJgQ&gt;`_</t>
+  </si>
+  <si>
+    <t>Distributed Computing, Part 1</t>
+  </si>
+  <si>
+    <t>Distributed Computing, Part 2</t>
+  </si>
+  <si>
+    <t>- Data Science: Backwards Design
+- Regular Expressions</t>
+  </si>
+  <si>
+    <t>- Parallelism
+- Defining Your Own Estimators</t>
+  </si>
+  <si>
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
-- Review Linear Regression Matrix Algebra
-- Review Defining Classes</t>
-  </si>
-  <si>
-    <t>Statsmodels Day 2</t>
+- Review linear regression as matrix manipulations. `Here's a nice review. &lt;https://www.stat.purdue.edu/~boli/stat512/lectures/topic3.pdf&gt;`_
+- `Review how to define classes &lt;https://realpython.com/python3-object-oriented-programming/&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -757,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,7 +786,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -782,12 +795,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -798,161 +811,161 @@
     </row>
     <row r="3" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -960,176 +973,187 @@
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" t="s">
         <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="113" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" t="s">
         <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="99" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="9" t="s">
+    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
         <v>99</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C27" s="9" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update class schedule links
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6C9CFF-3A28-A348-9F31-AC288E50DF9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D673CB-8E42-B347-B44B-4690B8CF438F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -356,15 +356,7 @@
     <t>Statsmodels Day 2</t>
   </si>
   <si>
-    <t>Regular Expressions</t>
-  </si>
-  <si>
     <t>- `Regular Expressions Tutorial &lt;https://scotch.io/tutorials/an-introduction-to-regex-in-python&gt;`_</t>
-  </si>
-  <si>
-    <t>- `Parallel ML with Dask &lt;https://www.youtube.com/watch?v=tQBovBvSDvA&amp;list=PLsT4-aZA6_bgaRhsc0JaZXSi5kt-RIJgQ&gt;`_
-- `What is Dask? &lt;scaling_parallelism_and_distributedcomputing.ipynb&gt;`_
-- `OPTIONAL: Full Dask Tutorial (3+ Hours) &lt;https://www.youtube.com/watch?v=mqdglv9GnM8&amp;list=PLsT4-aZA6_bgaRhsc0JaZXSi5kt-RIJgQ&gt;`_</t>
   </si>
   <si>
     <t>Distributed Computing, Part 1</t>
@@ -384,6 +376,12 @@
     <t>- `Parallel Computing &lt;parallelism.ipynb&gt;`_
 - Review linear regression as matrix manipulations. `Here's a nice review. &lt;https://www.stat.purdue.edu/~boli/stat512/lectures/topic3.pdf&gt;`_
 - `Review how to define classes &lt;https://realpython.com/python3-object-oriented-programming/&gt;`_</t>
+  </si>
+  <si>
+    <t>- `Distributed Computing with dask &lt;distributed_computing.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;https://www.practicaldatascience.org/html/distributed_computing.html#Exercises&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -770,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B7305-17E2-2E47-A46F-9F5E56C2016C}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1104,10 +1102,10 @@
         <v>80</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
         <v>94</v>
@@ -1118,21 +1116,24 @@
         <v>81</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>98</v>
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,7 +1141,7 @@
         <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1149,11 +1150,6 @@
       </c>
       <c r="B29" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dask exercises and solutions
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D673CB-8E42-B347-B44B-4690B8CF438F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE0FD78-4060-654B-B696-D8A6FE9C7E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
@@ -381,7 +381,7 @@
     <t>- `Distributed Computing with dask &lt;distributed_computing.ipynb&gt;`_</t>
   </si>
   <si>
-    <t>`Link &lt;https://www.practicaldatascience.org/html/distributed_computing.html#Exercises&gt;`_</t>
+    <t>`Link &lt;exercises/Exercise_dask.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
dask day two exercises
</commit_message>
<xml_diff>
--- a/source/class_schedule_xlsx.xlsx
+++ b/source/class_schedule_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nick/github/practicaldatascience/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE0FD78-4060-654B-B696-D8A6FE9C7E45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F622A7-9B48-BB42-A8E3-86E33D89880E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
+    <workbookView xWindow="7460" yWindow="1720" windowWidth="25600" windowHeight="14520" xr2:uid="{212B26BE-C12B-1745-A277-D3917F547107}"/>
   </bookViews>
   <sheets>
     <sheet name="class_schedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Topic</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>`Link &lt;exercises/Exercise_dask.ipynb&gt;`_</t>
+  </si>
+  <si>
+    <t>`Link &lt;exercises/Exercise_dask_realdata.ipynb&gt;`_</t>
   </si>
 </sst>
 </file>
@@ -771,7 +774,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,6 +1146,9 @@
       <c r="B28" t="s">
         <v>98</v>
       </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">

</xml_diff>